<commit_message>
feat : ajout des obstacles + score
J'ai ajouté la fonctionnalité de pouvoir placer des murs (au max 5) en appuyant sur la touche E, j'ai de plus ajouté le score. Chaque fois que un ennemi est tué cela rajoute 10 de score.
</commit_message>
<xml_diff>
--- a/J320-thoreynaud-jdt.xlsx
+++ b/J320-thoreynaud-jdt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk84vtk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2e\POO\Shoot-em-UP-2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278DAAD8-5C54-46C2-9187-BA3881C39794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384106FF-C5EF-4176-80A8-195882D8D01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t xml:space="preserve">Journal de travail + github       </t>
+  </si>
+  <si>
+    <t>Le prof nous a introduit le projet, finalement nous allons faire un jeux vidéo de notre choix dans le style space invaders</t>
+  </si>
+  <si>
+    <t>J'ai pris connaisance du Cdc et j'ai decider où m'orienter, dans quel style de jeux je veux partir</t>
+  </si>
+  <si>
+    <t>J'ai créer mon repo github avec le projet comme demandé par le prof, et j'ai ensuite crer mon projet en partant de la base. Cela ne me convenait pas alors j'ai changé pour partir sur le framework monogame.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai remplis mon journal de travail avec les actions effectuée aujourd'hui </t>
+  </si>
+  <si>
+    <t>Docummentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal de travail       </t>
   </si>
 </sst>
 </file>
@@ -444,6 +462,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -455,40 +507,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -811,7 +829,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -829,10 +847,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="33"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -844,10 +862,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -859,10 +877,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -874,12 +892,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -902,39 +920,59 @@
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="24">
         <v>45929</v>
       </c>
       <c r="C6" s="5">
+        <v>90</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="8">
         <v>45</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="8">
+        <v>30</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="8">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
-      <c r="B10" s="30"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -943,16 +981,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="24">
         <v>45930</v>
       </c>
       <c r="C12" s="5">
@@ -967,7 +1005,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="8">
         <v>45</v>
       </c>
@@ -980,7 +1018,7 @@
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="8">
         <v>20</v>
       </c>
@@ -991,14 +1029,14 @@
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="29"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
-      <c r="B16" s="30"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="10"/>
@@ -1007,42 +1045,44 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="28"/>
+      <c r="B18" s="24">
+        <v>45936</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="29"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="29"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="29"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
-      <c r="B22" s="30"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="10"/>
@@ -1051,42 +1091,44 @@
       <c r="A23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="28"/>
+      <c r="B24" s="24">
+        <v>45937</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="29"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="29"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="29"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="10"/>
       <c r="D28" s="11"/>
       <c r="E28" s="10"/>
@@ -1095,42 +1137,44 @@
       <c r="A29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-      <c r="B30" s="28"/>
+      <c r="B30" s="24">
+        <v>45957</v>
+      </c>
       <c r="C30" s="13"/>
       <c r="D30" s="14"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="29"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="29"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
-      <c r="B34" s="30"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
@@ -1139,42 +1183,44 @@
       <c r="A35" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="29"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="34"/>
+      <c r="B36" s="24">
+        <v>45958</v>
+      </c>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="29"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="29"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
-      <c r="B40" s="30"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="10"/>
       <c r="D40" s="11"/>
       <c r="E40" s="10"/>
@@ -1183,42 +1229,42 @@
       <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="29"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="29"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="29"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
-      <c r="B46" s="30"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="10"/>
       <c r="D46" s="11"/>
       <c r="E46" s="10"/>
@@ -1227,42 +1273,42 @@
       <c r="A47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="33"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
-      <c r="B48" s="28"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="29"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="29"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="29"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="30"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1271,42 +1317,42 @@
       <c r="A53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="33"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
-      <c r="B54" s="28"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="5"/>
       <c r="D54" s="6"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="29"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="8"/>
       <c r="D55" s="9"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="29"/>
+      <c r="B56" s="25"/>
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="29"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10"/>
-      <c r="B58" s="30"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
@@ -1315,42 +1361,42 @@
       <c r="A59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="33"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
-      <c r="B60" s="28"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="13"/>
       <c r="D60" s="14"/>
       <c r="E60" s="13"/>
     </row>
     <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
-      <c r="B61" s="29"/>
+      <c r="B61" s="25"/>
       <c r="C61" s="8"/>
       <c r="D61" s="9"/>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
-      <c r="B62" s="29"/>
+      <c r="B62" s="25"/>
       <c r="C62" s="8"/>
       <c r="D62" s="9"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="29"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
-      <c r="B64" s="30"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
@@ -1359,19 +1405,19 @@
       <c r="A65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="33"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="29"/>
     </row>
     <row r="66" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="36"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="15">
         <f>MROUND(SUM(C6:C65) /60,0.2)</f>
-        <v>4.6000000000000005</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="D66" s="16"/>
       <c r="E66" s="17"/>
@@ -1386,15 +1432,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:E59"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1411,6 +1448,15 @@
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:B34"/>
     <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="B59:E59"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C54:C58 C48:C52 C36:C40 C42:C46 C18:C22 B6 C12:C16 C24:C28 C30:C34 C60:C64 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1432,6 +1478,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010001B83F0F57411444B7FFB6944C19754C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="1902e5673cde7d7b1059ab5b9621db60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f910b7e-5659-40b0-877b-7416054d0d55" xmlns:ns3="766e0ef3-9166-4cc7-bffc-e6afe7b523a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cf0a760d7c5c5580796dd9be87835f4" ns2:_="" ns3:_="">
     <xsd:import namespace="7f910b7e-5659-40b0-877b-7416054d0d55"/>
@@ -1632,15 +1687,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1654,6 +1700,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10E1F6F4-11E8-48B3-A280-0CBC9F0440B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1672,14 +1726,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>